<commit_message>
Bedingte Formatierung in Excel Sheet
</commit_message>
<xml_diff>
--- a/Testfälle.xlsx
+++ b/Testfälle.xlsx
@@ -221,7 +221,68 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -499,7 +560,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="104" zoomScaleNormal="104" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -775,6 +838,17 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:C25">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="zu testen">
+      <formula>NOT(ISERROR(SEARCH("zu testen",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="ok">
+      <formula>NOT(ISERROR(SEARCH("ok",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="fehlerhaft">
+      <formula>NOT(ISERROR(SEARCH("fehlerhaft",C2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Kundenwechsel Begrenzung möglicher IDs nach oben
</commit_message>
<xml_diff>
--- a/Testfälle.xlsx
+++ b/Testfälle.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t>Beschreibung</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>zu testen</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -221,27 +224,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -259,16 +242,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -560,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -774,7 +747,7 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -794,7 +767,7 @@
         <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
@@ -839,13 +812,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C25">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="zu testen">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="zu testen">
       <formula>NOT(ISERROR(SEARCH("zu testen",C2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="ok">
       <formula>NOT(ISERROR(SEARCH("ok",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="fehlerhaft">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="fehlerhaft">
       <formula>NOT(ISERROR(SEARCH("fehlerhaft",C2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Kunden-ID bei Erstellung mitgeben
</commit_message>
<xml_diff>
--- a/Testfälle.xlsx
+++ b/Testfälle.xlsx
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -694,7 +694,7 @@
         <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Neueingabe bei falscher Zeitangabe erzwingen
</commit_message>
<xml_diff>
--- a/Testfälle.xlsx
+++ b/Testfälle.xlsx
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -716,7 +716,7 @@
         <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -727,7 +727,7 @@
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
ausleihePreis abhängig von menge
</commit_message>
<xml_diff>
--- a/Testfälle.xlsx
+++ b/Testfälle.xlsx
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -793,7 +793,7 @@
         <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Handling-Pauschale wird bei Verlust nicht fällig
</commit_message>
<xml_diff>
--- a/Testfälle.xlsx
+++ b/Testfälle.xlsx
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -804,7 +804,7 @@
         <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Testfälle um Beschreibung des Vorgehens erweitert
</commit_message>
<xml_diff>
--- a/Testfälle.xlsx
+++ b/Testfälle.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="76">
   <si>
     <t>Beschreibung</t>
   </si>
@@ -177,6 +177,81 @@
   </si>
   <si>
     <t>Zeitpunkt fehlt bei Verkäufen und abgeschlossen Ausleihen</t>
+  </si>
+  <si>
+    <t>Vorgehensbeschreibung</t>
+  </si>
+  <si>
+    <t>Liste zum Verkaufen: Taste 3; Liste zum Verleihen: Taste 5</t>
+  </si>
+  <si>
+    <t>Verkaufen mit Taste 4; Verleihen mit Taste 6 - Dann Listen aufrufen nach D2</t>
+  </si>
+  <si>
+    <t>Liste zum Verkaufen: Taste 1; Liste zum Verleihen: Taste 2</t>
+  </si>
+  <si>
+    <t>Verkaufen mit Taste 4; Verleihen mit Taste 6 - Dann Listen aufrufen nach D4</t>
+  </si>
+  <si>
+    <t>Analog zu D5, hier auch absichtliche Falscheingaben (zu hohe Menge, negative Menge)</t>
+  </si>
+  <si>
+    <t>Rückgabe mit Taste 7</t>
+  </si>
+  <si>
+    <t>Rückgabe mit Taste 7 - Mengeneingabe höher als ausgeliehene Menge</t>
+  </si>
+  <si>
+    <t>Nach einem Verkauf oder einer Rückgabe / Verlustmeldung: Abrechnung mit Taste 9 - Kontrolle in Transaktionsbericht mit Taste 11</t>
+  </si>
+  <si>
+    <t>Nach erfolgreicher Abrechnung: Umsatzbericht mit Taste 9 - Kontrolle in Transaktionsbericht mit Taste 11</t>
+  </si>
+  <si>
+    <t>Nach einem Verkauf oder einer Rückgabe / Verlustmeldung: Transaktionsbericht mit Taste 11</t>
+  </si>
+  <si>
+    <t>Kundendaten ändern mit Taste 13 - Kontrolle der Datenänderung in Übersicht mit Taste 0</t>
+  </si>
+  <si>
+    <t>Neuen Kunden anlegen mit Taste 12 - Kontrolle in Umsatzbericht, ob der neue Kunde aufgeführt wird</t>
+  </si>
+  <si>
+    <t>Verkaufen mit Taste 4 - Eingabe einer Produkt-ID die nicht in der Liste der verkäuflichen Gegenstände aufgeführt wird, aber im Produktsortiment vertreten ist</t>
+  </si>
+  <si>
+    <t>Bestätigung der Datenänderung</t>
+  </si>
+  <si>
+    <t>Fehlermeldung bei Verlustmeldung - keine Datenänderung</t>
+  </si>
+  <si>
+    <t>Direkte Zahlungsaufforderung nach Verkauf von Dienstleistungen</t>
+  </si>
+  <si>
+    <t>Protokoll</t>
+  </si>
+  <si>
+    <t>Zeit ändern mit Taste 15 - Eingabe einer negativen Zahl</t>
+  </si>
+  <si>
+    <t>Zeit ändern mit Taste 15 - Eingabe einer positiven Zahl</t>
+  </si>
+  <si>
+    <t>Verleihen mit Taste 6 - Zeit ändern mit Taste 15, dabei eine andere Zeit angeben als die der prognostizierten Zeitdauer der Ausleihe - Rückgabe mit Taste 7 - Vergleich der zu zahlenden Summe mit einer Rechnung von Hand</t>
+  </si>
+  <si>
+    <t>Kunden wechseln mit Taste 14 - Kontrolle des aktuellen Kunden in Übersicht mit Taste 0</t>
+  </si>
+  <si>
+    <t>Verkaufen mit Taste 4 - Eingabe einer Produkt-ID einer Dienstleistung (Beispielsweise 15 für eine Hallenreinigung) - Keine Bestandsänderung (unendliche Menge im Rahmen von INT.MAX_VALUE möglich)</t>
+  </si>
+  <si>
+    <t>Verleih mit Taste 6: Produkt-ID 7 für Toilettenwagen - Verlust melden mit Taste 7 - Fehlermeldung bei Bestätigung</t>
+  </si>
+  <si>
+    <t>Verkauf mit Taste 4: Produkt-ID 15 für Hallenreinigung oder eine andere Dienstleistung - Zahlungsaufforderung erscheint (Kontrolle: Transaktion erscheint ohne manuelle Abrechnung in dem Bericht mit Taste 11)</t>
   </si>
 </sst>
 </file>
@@ -208,7 +283,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -216,16 +291,112 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -233,11 +404,11 @@
   <dxfs count="3">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -253,11 +424,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -537,19 +708,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="82.08984375" customWidth="1"/>
-    <col min="2" max="2" width="81.81640625" customWidth="1"/>
+    <col min="1" max="1" width="56.26953125" customWidth="1"/>
+    <col min="2" max="2" width="61" customWidth="1"/>
+    <col min="4" max="4" width="49.7265625" customWidth="1"/>
+    <col min="5" max="5" width="50.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,276 +730,379 @@
       <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="C3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="C4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="C5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="C6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="C7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="C8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="C9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="C10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="C11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="C13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="C14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="9" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="C16" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="C17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="C18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="B19" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="C21" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="C22" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+      <c r="C23" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="10"/>
+      <c r="E23" s="11"/>
+    </row>
+    <row r="24" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
+      <c r="B24" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" t="s">
-        <v>48</v>
-      </c>
+      <c r="B25" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="11"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C25">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="zu testen">
-      <formula>NOT(ISERROR(SEARCH("zu testen",C2)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="fehlerhaft">
+      <formula>NOT(ISERROR(SEARCH("fehlerhaft",C2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="ok">
       <formula>NOT(ISERROR(SEARCH("ok",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="fehlerhaft">
-      <formula>NOT(ISERROR(SEARCH("fehlerhaft",C2)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="zu testen">
+      <formula>NOT(ISERROR(SEARCH("zu testen",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>